<commit_message>
data extraction done for single page
</commit_message>
<xml_diff>
--- a/Writing to Excel.xlsx
+++ b/Writing to Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/pa0005in_e_ntu_edu_sg/Documents/Trim3/AN6817 RPA/Projects/DataCentreCalculator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_29CED34F86A7969D1E54189E91BA69E66D3BCEA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F7B8721-831A-49E7-A4C1-75907DFCF481}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7317CDAB-8A57-4252-836F-8CC920C2B40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <x:si>
     <x:t>DATA CENTER CAPITAL COST CALCULATOR</x:t>
   </x:si>
@@ -41,6 +41,99 @@
   </x:si>
   <x:si>
     <x:t>Location of Data Center</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Center Environment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Center Design Capacity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cooling System</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Air distribution type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UPS Architecture</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Power distribution type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Power Density</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Core &amp; shell</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 kW / rack</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$ 90 / hour</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$ 90 / ft²</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Labor Rate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Redundancy Level</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Power</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cooling</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT distribution</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UPS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Generator</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Capital Cost Summary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$ 7.2 M</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Center Cost</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Data Center Cost Per Watt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$ 7.19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Calculated Rack Quantity</x:t>
+  </x:si>
+  <x:si>
+    <x:t>250</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT Room Area</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8,125 ft²</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Facility Area</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,195 ft²</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cost by Type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cost by System</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -372,35 +465,190 @@
   </x:sheetPr>
   <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F10" sqref="F10 1:1048576"/>
+    <x:sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <x:selection activeCell="A22" sqref="A22 A1:A36"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:1">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
+    <x:row r="2" spans="1:1">
       <x:c r="A2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:6">
+    <x:row r="3" spans="1:1">
       <x:c r="A3" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:6">
+    <x:row r="4" spans="1:1">
       <x:c r="A4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:6">
+    <x:row r="5" spans="1:1">
       <x:c r="A5" s="0" t="s">
         <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1">
+      <x:c r="A6" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1">
+      <x:c r="A7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:1">
+      <x:c r="A8" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:1">
+      <x:c r="A9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:1">
+      <x:c r="A10" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:1">
+      <x:c r="A11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:1">
+      <x:c r="A12" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:1">
+      <x:c r="A13" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:1">
+      <x:c r="A14" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:1">
+      <x:c r="A15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:1">
+      <x:c r="A16" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:1">
+      <x:c r="A17" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:1">
+      <x:c r="A18" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:1">
+      <x:c r="A19" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:1">
+      <x:c r="A20" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:1">
+      <x:c r="A21" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:1">
+      <x:c r="A22" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:1">
+      <x:c r="A23" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:1">
+      <x:c r="A24" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:1">
+      <x:c r="A25" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:1">
+      <x:c r="A26" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:1">
+      <x:c r="A27" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:1">
+      <x:c r="A28" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:1">
+      <x:c r="A29" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:1">
+      <x:c r="A30" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:1">
+      <x:c r="A31" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:1">
+      <x:c r="A32" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:1">
+      <x:c r="A33" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:1">
+      <x:c r="A34" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:1">
+      <x:c r="A35" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:1">
+      <x:c r="A36" s="0" t="s">
+        <x:v>35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>